<commit_message>
Added in fancy stats boxes and deployed server
</commit_message>
<xml_diff>
--- a/server/Report.xlsx
+++ b/server/Report.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>Last Name</t>
   </si>
@@ -111,6 +111,12 @@
     <t>Yann Martel</t>
   </si>
   <si>
+    <t>Rationality: from AI to Zombies</t>
+  </si>
+  <si>
+    <t>Eliezer Yudkowsky</t>
+  </si>
+  <si>
     <t>Smart People Should Build Things</t>
   </si>
   <si>
@@ -157,6 +163,15 @@
   </si>
   <si>
     <t>Rogg, Sebastian</t>
+  </si>
+  <si>
+    <t>W7CPzamcGj</t>
+  </si>
+  <si>
+    <t>Yudkowsky, Eliezer</t>
+  </si>
+  <si>
+    <t>we1zhU2xyb</t>
   </si>
 </sst>
 </file>
@@ -347,7 +362,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -357,7 +372,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -416,7 +431,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -427,10 +442,10 @@
         <v>35</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -441,9 +456,23 @@
         <v>37</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -454,7 +483,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -462,13 +491,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -476,43 +505,65 @@
         <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>